<commit_message>
[➕Add] Stage improve - ui feature add
- 적 공격력과 골드 상승 분리
- 플레이어 체력 변경 함수 공개로 수정, 보스 클리어 시 체력 초기화
- 진행 상황 게이지 조절기능 추가 및 ui 새로고침 전반적으로 수정
- 테이블 생성에 맞춰 몬스터 능력치 임시 조정
</commit_message>
<xml_diff>
--- a/IdleGame/Assets/Resources/ExcelTable/StageTable.xlsx
+++ b/IdleGame/Assets/Resources/ExcelTable/StageTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F27CB41-406C-4873-8C29-C1F77EB6EFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A82AF08-37F0-4419-9DC9-E1C1A55CD23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8850" yWindow="1350" windowWidth="17205" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,10 +51,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>EnemyStatRage : Int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>EnemyGoldRate : Int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -147,6 +143,10 @@
   </si>
   <si>
     <t>2-10</t>
+  </si>
+  <si>
+    <t>EnemyStatRate : Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -276,9 +276,9 @@
     <tableColumn id="3" xr3:uid="{771CEA38-D7C4-4046-BF0E-BCAC6EBCCFF5}" name="Chapter : String" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{9A52DE84-B46A-41BA-9891-9221E6FD8CA2}" name="StageConfig : String" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{52BABBB3-0B5B-4EA5-A096-52FE17505682}" name="StageBackground : String" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{8CB87B44-9BE8-4447-B7A9-5AB6AF555193}" name="EnemyStatRage : Int" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{8CB87B44-9BE8-4447-B7A9-5AB6AF555193}" name="EnemyStatRate : Int" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{70C60707-1493-4007-90DF-8D1A8171AA79}" name="EnemyGoldRate : Int" dataDxfId="1">
-      <calculatedColumnFormula>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</calculatedColumnFormula>
+      <calculatedColumnFormula>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{A1894453-017C-4920-B6D4-6CCC399479DE}" name="EnemySpawnCount : Int" dataDxfId="0"/>
   </tableColumns>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -589,13 +589,13 @@
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -603,20 +603,20 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2">
         <v>10</v>
       </c>
       <c r="G3" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>8</v>
       </c>
       <c r="H3" s="2">
@@ -628,20 +628,20 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2">
         <v>15</v>
       </c>
       <c r="G4" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>12</v>
       </c>
       <c r="H4" s="2">
@@ -653,20 +653,20 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2">
         <v>20</v>
       </c>
       <c r="G5" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>16</v>
       </c>
       <c r="H5" s="2">
@@ -678,20 +678,20 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2">
         <v>25</v>
       </c>
       <c r="G6" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>20</v>
       </c>
       <c r="H6" s="2">
@@ -703,20 +703,20 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2">
         <v>40</v>
       </c>
       <c r="G7" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>32</v>
       </c>
       <c r="H7" s="2">
@@ -728,20 +728,20 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2">
         <v>45</v>
       </c>
       <c r="G8" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>36</v>
       </c>
       <c r="H8" s="2">
@@ -753,20 +753,20 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2">
         <v>50</v>
       </c>
       <c r="G9" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>40</v>
       </c>
       <c r="H9" s="2">
@@ -778,20 +778,20 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2">
         <v>55</v>
       </c>
       <c r="G10" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>44</v>
       </c>
       <c r="H10" s="2">
@@ -803,20 +803,20 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2">
         <v>60</v>
       </c>
       <c r="G11" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>48</v>
       </c>
       <c r="H11" s="2">
@@ -828,20 +828,20 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
         <v>80</v>
       </c>
       <c r="G12" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>64</v>
       </c>
       <c r="H12" s="2">
@@ -853,20 +853,20 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
         <v>90</v>
       </c>
       <c r="G13" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>72</v>
       </c>
       <c r="H13" s="2">
@@ -878,20 +878,20 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2">
         <v>100</v>
       </c>
       <c r="G14" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>80</v>
       </c>
       <c r="H14" s="2">
@@ -903,20 +903,20 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2">
         <v>110</v>
       </c>
       <c r="G15" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>88</v>
       </c>
       <c r="H15" s="2">
@@ -928,20 +928,20 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2">
         <v>120</v>
       </c>
       <c r="G16" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>96</v>
       </c>
       <c r="H16" s="2">
@@ -953,20 +953,20 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2">
         <v>150</v>
       </c>
       <c r="G17" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>120</v>
       </c>
       <c r="H17" s="2">
@@ -978,20 +978,20 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2">
         <v>160</v>
       </c>
       <c r="G18" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>128</v>
       </c>
       <c r="H18" s="2">
@@ -1003,20 +1003,20 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2">
         <v>170</v>
       </c>
       <c r="G19" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>136</v>
       </c>
       <c r="H19" s="2">
@@ -1028,20 +1028,20 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2">
         <v>185</v>
       </c>
       <c r="G20" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>148</v>
       </c>
       <c r="H20" s="2">
@@ -1053,20 +1053,20 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2">
         <v>200</v>
       </c>
       <c r="G21" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>160</v>
       </c>
       <c r="H21" s="2">
@@ -1078,20 +1078,20 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2">
         <v>250</v>
       </c>
       <c r="G22" s="2">
-        <f>ROUNDUP(표1[[#This Row],[EnemyStatRage : Int]]*0.8,0)</f>
+        <f>ROUNDUP(표1[[#This Row],[EnemyStatRate : Int]]*0.8,0)</f>
         <v>200</v>
       </c>
       <c r="H22" s="2">

</xml_diff>